<commit_message>
update issue with scaling
</commit_message>
<xml_diff>
--- a/Midterm Project/Feature_description.xlsx
+++ b/Midterm Project/Feature_description.xlsx
@@ -1299,8 +1299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>